<commit_message>
added cluster analysis file
</commit_message>
<xml_diff>
--- a/OQ_PQ/WormSource_v3.0/WormExp_info.xlsx
+++ b/OQ_PQ/WormSource_v3.0/WormExp_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bioinformatics\Projects\WormExp\GitHub\OQ_PQ\WormSource_v3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE30105-2359-4CA2-8328-A6A0392352EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDBD03D-E2A3-4FBB-9848-67E62152EB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16020" yWindow="1080" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17259" uniqueCount="3830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17271" uniqueCount="3830">
   <si>
     <t>WormBaseVersion_checked</t>
   </si>
@@ -12213,27 +12213,7 @@
     <cellStyle name="常规 14" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="常规 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -12566,8 +12546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C1170" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F1222" sqref="F1222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -45345,7 +45325,9 @@
       <c r="F1105" s="2" t="s">
         <v>2729</v>
       </c>
-      <c r="G1105" s="2"/>
+      <c r="G1105" s="2" t="s">
+        <v>2729</v>
+      </c>
       <c r="H1105" s="2"/>
       <c r="I1105" s="2" t="s">
         <v>2952</v>
@@ -45417,7 +45399,9 @@
       <c r="F1108" s="2" t="s">
         <v>2729</v>
       </c>
-      <c r="G1108" s="2"/>
+      <c r="G1108" s="2" t="s">
+        <v>2729</v>
+      </c>
       <c r="H1108" s="2"/>
       <c r="I1108" s="2" t="s">
         <v>2952</v>
@@ -47001,7 +46985,9 @@
       <c r="F1174" s="2" t="s">
         <v>2729</v>
       </c>
-      <c r="G1174" s="2"/>
+      <c r="G1174" s="2" t="s">
+        <v>2729</v>
+      </c>
       <c r="H1174" s="2"/>
       <c r="I1174" s="2" t="s">
         <v>2961</v>
@@ -47025,7 +47011,9 @@
       <c r="F1175" s="2" t="s">
         <v>2729</v>
       </c>
-      <c r="G1175" s="2"/>
+      <c r="G1175" s="2" t="s">
+        <v>2729</v>
+      </c>
       <c r="H1175" s="2"/>
       <c r="I1175" s="2" t="s">
         <v>2961</v>
@@ -47241,7 +47229,9 @@
       <c r="F1184" s="2" t="s">
         <v>2747</v>
       </c>
-      <c r="G1184" s="2"/>
+      <c r="G1184" s="2" t="s">
+        <v>2747</v>
+      </c>
       <c r="H1184" s="2"/>
       <c r="I1184" s="2" t="s">
         <v>2964</v>
@@ -47265,7 +47255,9 @@
       <c r="F1185" s="2" t="s">
         <v>2747</v>
       </c>
-      <c r="G1185" s="2"/>
+      <c r="G1185" s="2" t="s">
+        <v>2747</v>
+      </c>
       <c r="H1185" s="2"/>
       <c r="I1185" s="2" t="s">
         <v>2964</v>
@@ -47289,7 +47281,9 @@
       <c r="F1186" s="2" t="s">
         <v>2748</v>
       </c>
-      <c r="G1186" s="2"/>
+      <c r="G1186" s="2" t="s">
+        <v>2748</v>
+      </c>
       <c r="H1186" s="2"/>
       <c r="I1186" s="2" t="s">
         <v>2965</v>
@@ -47313,7 +47307,9 @@
       <c r="F1187" s="2" t="s">
         <v>2748</v>
       </c>
-      <c r="G1187" s="2"/>
+      <c r="G1187" s="2" t="s">
+        <v>2748</v>
+      </c>
       <c r="H1187" s="2"/>
       <c r="I1187" s="2" t="s">
         <v>2965</v>
@@ -47337,7 +47333,9 @@
       <c r="F1188" s="2" t="s">
         <v>2748</v>
       </c>
-      <c r="G1188" s="2"/>
+      <c r="G1188" s="2" t="s">
+        <v>2748</v>
+      </c>
       <c r="H1188" s="2"/>
       <c r="I1188" s="2" t="s">
         <v>2965</v>
@@ -47361,7 +47359,9 @@
       <c r="F1189" s="2" t="s">
         <v>2748</v>
       </c>
-      <c r="G1189" s="2"/>
+      <c r="G1189" s="2" t="s">
+        <v>2748</v>
+      </c>
       <c r="H1189" s="2"/>
       <c r="I1189" s="2" t="s">
         <v>2965</v>
@@ -47385,7 +47385,9 @@
       <c r="F1190" s="2" t="s">
         <v>2748</v>
       </c>
-      <c r="G1190" s="2"/>
+      <c r="G1190" s="2" t="s">
+        <v>2748</v>
+      </c>
       <c r="H1190" s="2"/>
       <c r="I1190" s="2" t="s">
         <v>2965</v>
@@ -47409,7 +47411,9 @@
       <c r="F1191" s="2" t="s">
         <v>2748</v>
       </c>
-      <c r="G1191" s="2"/>
+      <c r="G1191" s="2" t="s">
+        <v>2748</v>
+      </c>
       <c r="H1191" s="2"/>
       <c r="I1191" s="2" t="s">
         <v>2965</v>

</xml_diff>